<commit_message>
Crear Script de tabla basicas de Ejecucion del sistema, diferentes a las del archivo de excel Agregar al excel la patbla Packaging (Embalajes)
</commit_message>
<xml_diff>
--- a/documentos/Formato definicion poblado inicial de tablas de parametrizacion Aldebaran.xlsx
+++ b/documentos/Formato definicion poblado inicial de tablas de parametrizacion Aldebaran.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="4680" windowWidth="14805" windowHeight="8010" tabRatio="801" firstSheet="21" activeTab="29"/>
+    <workbookView xWindow="240" yWindow="5595" windowWidth="14805" windowHeight="8010" tabRatio="801" firstSheet="22" activeTab="31"/>
   </bookViews>
   <sheets>
     <sheet name="Descripcion del Archivo" sheetId="32" r:id="rId1"/>
@@ -38,13 +38,14 @@
     <sheet name="Proveedores" sheetId="28" r:id="rId29"/>
     <sheet name="Referencias por Proveedor" sheetId="29" r:id="rId30"/>
     <sheet name="Metodos de envio" sheetId="30" r:id="rId31"/>
+    <sheet name="Embalajes" sheetId="36" r:id="rId32"/>
   </sheets>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="386">
   <si>
     <t>*</t>
   </si>
@@ -1330,14 +1331,36 @@
   <si>
     <t>Redetrans</t>
   </si>
+  <si>
+    <t>Tamaño del empaque por Item</t>
+  </si>
+  <si>
+    <t>ITEM_ID, WEIGHT, HEIGHT, WIDTH, LENGTH, QUANTITY</t>
+  </si>
+  <si>
+    <t>packaging</t>
+  </si>
+  <si>
+    <t>Tamaño</t>
+  </si>
+  <si>
+    <t>Ancho</t>
+  </si>
+  <si>
+    <t>Alto</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000000000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1589,7 +1612,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1682,6 +1705,8 @@
     <xf numFmtId="49" fontId="11" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1706,14 +1731,75 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="215">
+  <dxfs count="224">
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -3113,39 +3199,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla11" displayName="Tabla11" ref="A5:A7" totalsRowShown="0" headerRowDxfId="214" dataDxfId="213" tableBorderDxfId="212">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabla11" displayName="Tabla11" ref="A5:A7" totalsRowShown="0" headerRowDxfId="223" dataDxfId="222" tableBorderDxfId="221">
   <tableColumns count="1">
-    <tableColumn id="1" name="Nombre de la actividad" dataDxfId="211"/>
+    <tableColumn id="1" name="Nombre de la actividad" dataDxfId="220"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tabla19" displayName="Tabla19" ref="A5:B8" totalsRowShown="0" headerRowDxfId="166" dataDxfId="165" tableBorderDxfId="164">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Tabla19" displayName="Tabla19" ref="A5:B8" totalsRowShown="0" headerRowDxfId="175" dataDxfId="174" tableBorderDxfId="173">
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre del Motivo" dataDxfId="163"/>
-    <tableColumn id="2" name="Descripción" dataDxfId="162"/>
+    <tableColumn id="1" name="Nombre del Motivo" dataDxfId="172"/>
+    <tableColumn id="2" name="Descripción" dataDxfId="171"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="A5:B7" totalsRowShown="0" headerRowDxfId="161" dataDxfId="160" tableBorderDxfId="159">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="A5:B7" totalsRowShown="0" headerRowDxfId="170" dataDxfId="169" tableBorderDxfId="168">
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre del País" dataDxfId="158"/>
-    <tableColumn id="2" name="Código del País" dataDxfId="157"/>
+    <tableColumn id="1" name="Nombre del País" dataDxfId="167"/>
+    <tableColumn id="2" name="Código del País" dataDxfId="166"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="A5:C8" totalsRowShown="0" headerRowDxfId="156">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="A5:C8" totalsRowShown="0" headerRowDxfId="165">
   <tableColumns count="3">
-    <tableColumn id="1" name="Nombre del Departamento" dataDxfId="155"/>
-    <tableColumn id="2" name="País" dataDxfId="154"/>
+    <tableColumn id="1" name="Nombre del Departamento" dataDxfId="164"/>
+    <tableColumn id="2" name="País" dataDxfId="163"/>
     <tableColumn id="3" name="Concatenado">
       <calculatedColumnFormula>IF(B6&lt;&gt;"",IF(A6&lt;&gt;"",CONCATENATE(B6,"-",A6),""),"")</calculatedColumnFormula>
     </tableColumn>
@@ -3155,11 +3241,11 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla17" displayName="Tabla17" ref="A5:C8" totalsRowShown="0" headerRowDxfId="153" tableBorderDxfId="152">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla17" displayName="Tabla17" ref="A5:C8" totalsRowShown="0" headerRowDxfId="162" tableBorderDxfId="161">
   <tableColumns count="3">
-    <tableColumn id="1" name="Nombre de la Ciudad" dataDxfId="151"/>
-    <tableColumn id="2" name="Departamento-Estado" dataDxfId="150"/>
-    <tableColumn id="6" name="Columna2" dataDxfId="149">
+    <tableColumn id="1" name="Nombre de la Ciudad" dataDxfId="160"/>
+    <tableColumn id="2" name="Departamento-Estado" dataDxfId="159"/>
+    <tableColumn id="6" name="Columna2" dataDxfId="158">
       <calculatedColumnFormula>IF(B6&lt;&gt;"",IF(A6&lt;&gt;"",CONCATENATE(B6,"-",A6),""),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3168,48 +3254,48 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="A5:B7" totalsRowShown="0" headerRowDxfId="148" dataDxfId="147" tableBorderDxfId="146">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabla7" displayName="Tabla7" ref="A5:B7" totalsRowShown="0" headerRowDxfId="157" dataDxfId="156" tableBorderDxfId="155">
   <tableColumns count="2">
-    <tableColumn id="1" name="Código del Tipo" dataDxfId="145"/>
-    <tableColumn id="2" name="Nombre del Tipo" dataDxfId="144"/>
+    <tableColumn id="1" name="Código del Tipo" dataDxfId="154"/>
+    <tableColumn id="2" name="Nombre del Tipo" dataDxfId="153"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="A5:J8" totalsRowShown="0" headerRowDxfId="143" dataDxfId="142" tableBorderDxfId="141">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabla8" displayName="Tabla8" ref="A5:J8" totalsRowShown="0" headerRowDxfId="152" dataDxfId="151" tableBorderDxfId="150">
   <tableColumns count="10">
-    <tableColumn id="1" name="Nombre del Satelite" dataDxfId="140"/>
-    <tableColumn id="2" name="Dirección del Satelite" dataDxfId="139"/>
-    <tableColumn id="3" name="Tipo de Identificación" dataDxfId="138"/>
-    <tableColumn id="4" name="Identificación" dataDxfId="137"/>
-    <tableColumn id="5" name="Teléfono" dataDxfId="136"/>
-    <tableColumn id="6" name="Fax" dataDxfId="135"/>
-    <tableColumn id="7" name="Email" dataDxfId="134"/>
-    <tableColumn id="8" name="Ciudad" dataDxfId="133"/>
-    <tableColumn id="9" name="Representante Legal" dataDxfId="132"/>
-    <tableColumn id="10" name="Activo" dataDxfId="131"/>
+    <tableColumn id="1" name="Nombre del Satelite" dataDxfId="149"/>
+    <tableColumn id="2" name="Dirección del Satelite" dataDxfId="148"/>
+    <tableColumn id="3" name="Tipo de Identificación" dataDxfId="147"/>
+    <tableColumn id="4" name="Identificación" dataDxfId="146"/>
+    <tableColumn id="5" name="Teléfono" dataDxfId="145"/>
+    <tableColumn id="6" name="Fax" dataDxfId="144"/>
+    <tableColumn id="7" name="Email" dataDxfId="143"/>
+    <tableColumn id="8" name="Ciudad" dataDxfId="142"/>
+    <tableColumn id="9" name="Representante Legal" dataDxfId="141"/>
+    <tableColumn id="10" name="Activo" dataDxfId="140"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A5:L7" totalsRowShown="0" tableBorderDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A5:L7" totalsRowShown="0" tableBorderDxfId="139">
   <tableColumns count="12">
-    <tableColumn id="1" name="Tipo de Identificación" dataDxfId="129"/>
-    <tableColumn id="2" name="Identificación" dataDxfId="128"/>
-    <tableColumn id="3" name="Nombre" dataDxfId="127"/>
-    <tableColumn id="4" name="Teléfono 1" dataDxfId="126"/>
-    <tableColumn id="5" name="Teléfono 2" dataDxfId="125"/>
-    <tableColumn id="6" name="Fax" dataDxfId="124"/>
-    <tableColumn id="7" name="Dirección" dataDxfId="123"/>
-    <tableColumn id="8" name="Celular" dataDxfId="122"/>
-    <tableColumn id="9" name="Correo Electrónico" dataDxfId="121" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="11" name="Ciudad" dataDxfId="120"/>
-    <tableColumn id="13" name="Envio de Correo" dataDxfId="119"/>
-    <tableColumn id="15" name="Columna4" dataDxfId="118">
+    <tableColumn id="1" name="Tipo de Identificación" dataDxfId="138"/>
+    <tableColumn id="2" name="Identificación" dataDxfId="137"/>
+    <tableColumn id="3" name="Nombre" dataDxfId="136"/>
+    <tableColumn id="4" name="Teléfono 1" dataDxfId="135"/>
+    <tableColumn id="5" name="Teléfono 2" dataDxfId="134"/>
+    <tableColumn id="6" name="Fax" dataDxfId="133"/>
+    <tableColumn id="7" name="Dirección" dataDxfId="132"/>
+    <tableColumn id="8" name="Celular" dataDxfId="131"/>
+    <tableColumn id="9" name="Correo Electrónico" dataDxfId="130" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="11" name="Ciudad" dataDxfId="129"/>
+    <tableColumn id="13" name="Envio de Correo" dataDxfId="128"/>
+    <tableColumn id="15" name="Columna4" dataDxfId="127">
       <calculatedColumnFormula>IF(A6&lt;&gt;"",IF(B6&lt;&gt;"",CONCATENATE(A6,"-",B6),""),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3218,48 +3304,48 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tabla20" displayName="Tabla20" ref="A5:E7" totalsRowShown="0" headerRowDxfId="117" dataDxfId="116" tableBorderDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Tabla20" displayName="Tabla20" ref="A5:E7" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125" tableBorderDxfId="124">
   <tableColumns count="5">
-    <tableColumn id="1" name="Cliente " dataDxfId="114"/>
-    <tableColumn id="2" name="Nombre del Contacto" dataDxfId="113"/>
-    <tableColumn id="3" name="Título" dataDxfId="112"/>
-    <tableColumn id="4" name="Teléfono" dataDxfId="111"/>
-    <tableColumn id="5" name="Correo Electrónico" dataDxfId="110" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="1" name="Cliente " dataDxfId="123"/>
+    <tableColumn id="2" name="Nombre del Contacto" dataDxfId="122"/>
+    <tableColumn id="3" name="Título" dataDxfId="121"/>
+    <tableColumn id="4" name="Teléfono" dataDxfId="120"/>
+    <tableColumn id="5" name="Correo Electrónico" dataDxfId="119" dataCellStyle="Hipervínculo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tabla2021" displayName="Tabla2021" ref="A5:H7" totalsRowShown="0" headerRowDxfId="109" dataDxfId="108" tableBorderDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tabla2021" displayName="Tabla2021" ref="A5:H7" totalsRowShown="0" headerRowDxfId="118" dataDxfId="117" tableBorderDxfId="116">
   <tableColumns count="8">
-    <tableColumn id="1" name="Nombre" dataDxfId="106"/>
-    <tableColumn id="2" name="Teléfono 1" dataDxfId="105"/>
-    <tableColumn id="3" name="Teléfono 2" dataDxfId="104"/>
-    <tableColumn id="4" name="Fax" dataDxfId="103"/>
-    <tableColumn id="9" name="Dirección" dataDxfId="102"/>
-    <tableColumn id="10" name="Correo Electrónico 1" dataDxfId="101"/>
-    <tableColumn id="7" name="Correo Electrónico 2" dataDxfId="100"/>
-    <tableColumn id="5" name="Ciudad " dataDxfId="99"/>
+    <tableColumn id="1" name="Nombre" dataDxfId="115"/>
+    <tableColumn id="2" name="Teléfono 1" dataDxfId="114"/>
+    <tableColumn id="3" name="Teléfono 2" dataDxfId="113"/>
+    <tableColumn id="4" name="Fax" dataDxfId="112"/>
+    <tableColumn id="9" name="Dirección" dataDxfId="111"/>
+    <tableColumn id="10" name="Correo Electrónico 1" dataDxfId="110"/>
+    <tableColumn id="7" name="Correo Electrónico 2" dataDxfId="109"/>
+    <tableColumn id="5" name="Ciudad " dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tabla202122" displayName="Tabla202122" ref="A5:K7" totalsRowShown="0" headerRowDxfId="98" tableBorderDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Tabla202122" displayName="Tabla202122" ref="A5:K7" totalsRowShown="0" headerRowDxfId="107" tableBorderDxfId="106">
   <tableColumns count="11">
-    <tableColumn id="1" name="Transportadora" dataDxfId="96"/>
-    <tableColumn id="2" name="Nombre" dataDxfId="95"/>
-    <tableColumn id="3" name="Teléfono 1" dataDxfId="94"/>
-    <tableColumn id="4" name="Teléfono 2" dataDxfId="93"/>
-    <tableColumn id="9" name="Fax" dataDxfId="92"/>
-    <tableColumn id="10" name="Dirección" dataDxfId="91"/>
-    <tableColumn id="7" name="Ciudad" dataDxfId="90"/>
-    <tableColumn id="12" name="Contacto" dataDxfId="89"/>
-    <tableColumn id="11" name="Correo Electrónico 1" dataDxfId="88" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="5" name="Correo Electrónico 2" dataDxfId="87"/>
-    <tableColumn id="13" name="Concatenado" dataDxfId="86">
+    <tableColumn id="1" name="Transportadora" dataDxfId="105"/>
+    <tableColumn id="2" name="Nombre" dataDxfId="104"/>
+    <tableColumn id="3" name="Teléfono 1" dataDxfId="103"/>
+    <tableColumn id="4" name="Teléfono 2" dataDxfId="102"/>
+    <tableColumn id="9" name="Fax" dataDxfId="101"/>
+    <tableColumn id="10" name="Dirección" dataDxfId="100"/>
+    <tableColumn id="7" name="Ciudad" dataDxfId="99"/>
+    <tableColumn id="12" name="Contacto" dataDxfId="98"/>
+    <tableColumn id="11" name="Correo Electrónico 1" dataDxfId="97" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="5" name="Correo Electrónico 2" dataDxfId="96"/>
+    <tableColumn id="13" name="Concatenado" dataDxfId="95">
       <calculatedColumnFormula>IF(A6&lt;&gt;"",IF(B6&lt;&gt;"",CONCATENATE(A6,"-",B6),""),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3268,87 +3354,87 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla9" displayName="Tabla9" ref="A5:C7" totalsRowShown="0" headerRowDxfId="210" dataDxfId="209" tableBorderDxfId="208">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabla9" displayName="Tabla9" ref="A5:C7" totalsRowShown="0" headerRowDxfId="219" dataDxfId="218" tableBorderDxfId="217">
   <tableColumns count="3">
-    <tableColumn id="1" name="Código del Area" dataDxfId="207"/>
-    <tableColumn id="2" name="Nombre del Area" dataDxfId="206"/>
-    <tableColumn id="3" name="Descripción" dataDxfId="205"/>
+    <tableColumn id="1" name="Código del Area" dataDxfId="216"/>
+    <tableColumn id="2" name="Nombre del Area" dataDxfId="215"/>
+    <tableColumn id="3" name="Descripción" dataDxfId="214"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tabla20212223" displayName="Tabla20212223" ref="A5:B9" totalsRowShown="0" headerRowDxfId="85" dataDxfId="84" tableBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Tabla20212223" displayName="Tabla20212223" ref="A5:B9" totalsRowShown="0" headerRowDxfId="94" dataDxfId="93" tableBorderDxfId="92">
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre del Método" dataDxfId="82"/>
-    <tableColumn id="2" name="Descripción " dataDxfId="81"/>
+    <tableColumn id="1" name="Nombre del Método" dataDxfId="91"/>
+    <tableColumn id="2" name="Descripción " dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tabla2021222324" displayName="Tabla2021222324" ref="A5:B7" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79" tableBorderDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Tabla2021222324" displayName="Tabla2021222324" ref="A5:B7" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88" tableBorderDxfId="87">
   <tableColumns count="2">
-    <tableColumn id="1" name="Metodo de Transporte" dataDxfId="77"/>
-    <tableColumn id="2" name="Agente de la Transportadora" dataDxfId="76"/>
+    <tableColumn id="1" name="Metodo de Transporte" dataDxfId="86"/>
+    <tableColumn id="2" name="Agente de la Transportadora" dataDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tabla202122232425" displayName="Tabla202122232425" ref="A5:D6" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74" tableBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24" name="Tabla202122232425" displayName="Tabla202122232425" ref="A5:D6" totalsRowShown="0" headerRowDxfId="84" dataDxfId="83" tableBorderDxfId="82">
   <tableColumns count="4">
-    <tableColumn id="1" name="Código" dataDxfId="72"/>
-    <tableColumn id="15" name="Nombre" dataDxfId="71"/>
-    <tableColumn id="14" name="Afecta la Pagina" dataDxfId="70"/>
-    <tableColumn id="2" name="Activa" dataDxfId="69"/>
+    <tableColumn id="1" name="Código" dataDxfId="81"/>
+    <tableColumn id="15" name="Nombre" dataDxfId="80"/>
+    <tableColumn id="14" name="Afecta la Pagina" dataDxfId="79"/>
+    <tableColumn id="2" name="Activa" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Tabla20212223242526" displayName="Tabla20212223242526" ref="A5:A8" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Tabla20212223242526" displayName="Tabla20212223242526" ref="A5:A8" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76" tableBorderDxfId="75">
   <tableColumns count="1">
-    <tableColumn id="1" name="Nombre" dataDxfId="65"/>
+    <tableColumn id="1" name="Nombre" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Tabla2021222324252627" displayName="Tabla2021222324252627" ref="A5:A9" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Tabla2021222324252627" displayName="Tabla2021222324252627" ref="A5:A9" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72" tableBorderDxfId="71">
   <tableColumns count="1">
-    <tableColumn id="1" name="Nombre" dataDxfId="61"/>
+    <tableColumn id="1" name="Nombre" dataDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Tabla20212223242528" displayName="Tabla20212223242528" ref="A5:R6" totalsRowShown="0" headerRowDxfId="60" tableBorderDxfId="59">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Tabla20212223242528" displayName="Tabla20212223242528" ref="A5:R6" totalsRowShown="0" headerRowDxfId="69" tableBorderDxfId="68">
   <tableColumns count="18">
-    <tableColumn id="1" name="Código de Linea" dataDxfId="58"/>
-    <tableColumn id="15" name="Referencia Interna" dataDxfId="57"/>
-    <tableColumn id="14" name="Nombre del Artículo" dataDxfId="56"/>
-    <tableColumn id="19" name="Reerencia para el proveedor" dataDxfId="55"/>
-    <tableColumn id="20" name="Nombre del Artículo para el Proveedor" dataDxfId="54"/>
-    <tableColumn id="21" name="Costo Fob" dataDxfId="53"/>
-    <tableColumn id="22" name="Moneda" dataDxfId="52"/>
-    <tableColumn id="17" name="Descripción" dataDxfId="51"/>
-    <tableColumn id="2" name="Inventario Externo" dataDxfId="50"/>
-    <tableColumn id="18" name="Costo Cif" dataDxfId="49"/>
-    <tableColumn id="27" name="Volumen" dataDxfId="48"/>
-    <tableColumn id="28" name="Peso" dataDxfId="47"/>
-    <tableColumn id="25" name="Unidad de medida Fob" dataDxfId="46"/>
-    <tableColumn id="26" name="Unidad de Medida Cif" dataDxfId="45"/>
-    <tableColumn id="23" name="Producto Nacional" dataDxfId="44"/>
-    <tableColumn id="24" name="Activo" dataDxfId="43"/>
-    <tableColumn id="16" name="Visible en el Catalogo Externo" dataDxfId="42"/>
-    <tableColumn id="29" name="Combinado" dataDxfId="41">
+    <tableColumn id="1" name="Código de Linea" dataDxfId="67"/>
+    <tableColumn id="15" name="Referencia Interna" dataDxfId="66"/>
+    <tableColumn id="14" name="Nombre del Artículo" dataDxfId="65"/>
+    <tableColumn id="19" name="Reerencia para el proveedor" dataDxfId="64"/>
+    <tableColumn id="20" name="Nombre del Artículo para el Proveedor" dataDxfId="63"/>
+    <tableColumn id="21" name="Costo Fob" dataDxfId="62"/>
+    <tableColumn id="22" name="Moneda" dataDxfId="61"/>
+    <tableColumn id="17" name="Descripción" dataDxfId="60"/>
+    <tableColumn id="2" name="Inventario Externo" dataDxfId="59"/>
+    <tableColumn id="18" name="Costo Cif" dataDxfId="58"/>
+    <tableColumn id="27" name="Volumen" dataDxfId="57"/>
+    <tableColumn id="28" name="Peso" dataDxfId="56"/>
+    <tableColumn id="25" name="Unidad de medida Fob" dataDxfId="55"/>
+    <tableColumn id="26" name="Unidad de Medida Cif" dataDxfId="54"/>
+    <tableColumn id="23" name="Producto Nacional" dataDxfId="53"/>
+    <tableColumn id="24" name="Activo" dataDxfId="52"/>
+    <tableColumn id="16" name="Visible en el Catalogo Externo" dataDxfId="51"/>
+    <tableColumn id="29" name="Combinado" dataDxfId="50">
       <calculatedColumnFormula>IF(A6&lt;&gt;"",IF(B6&lt;&gt;"",CONCATENATE(A6,"-",B6),""),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3357,29 +3443,29 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Tabla20212223242529" displayName="Tabla20212223242529" ref="A5:B6" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Tabla20212223242529" displayName="Tabla20212223242529" ref="A5:B6" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48" tableBorderDxfId="47">
   <tableColumns count="2">
-    <tableColumn id="1" name="Referencia Interna Artículo" dataDxfId="37"/>
-    <tableColumn id="15" name="Código del Area" dataDxfId="36"/>
+    <tableColumn id="1" name="Referencia Interna Artículo" dataDxfId="46"/>
+    <tableColumn id="15" name="Código del Area" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Tabla2021222324252930" displayName="Tabla2021222324252930" ref="A5:K6" totalsRowShown="0" headerRowDxfId="35" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Tabla2021222324252930" displayName="Tabla2021222324252930" ref="A5:K6" totalsRowShown="0" headerRowDxfId="44" tableBorderDxfId="43">
   <tableColumns count="11">
-    <tableColumn id="1" name="Referencia Interna artículo" dataDxfId="33"/>
-    <tableColumn id="24" name="Referencia" dataDxfId="32"/>
-    <tableColumn id="23" name="Referencia para el proveedor" dataDxfId="31"/>
-    <tableColumn id="22" name="Nombre de la referencia" dataDxfId="30"/>
-    <tableColumn id="21" name="Nombre de la referencia para el proveedor" dataDxfId="29"/>
-    <tableColumn id="20" name="Descripción" dataDxfId="28"/>
-    <tableColumn id="19" name="Cantidad en Bodega Local" dataDxfId="27"/>
-    <tableColumn id="18" name="Cantidad en Zona Franca" dataDxfId="26"/>
-    <tableColumn id="17" name="Activo" dataDxfId="25"/>
-    <tableColumn id="26" name="Cantidad Minima para Alarma" dataDxfId="24"/>
-    <tableColumn id="27" name="Combinado" dataDxfId="23">
+    <tableColumn id="1" name="Referencia Interna artículo" dataDxfId="42"/>
+    <tableColumn id="24" name="Referencia" dataDxfId="41"/>
+    <tableColumn id="23" name="Referencia para el proveedor" dataDxfId="40"/>
+    <tableColumn id="22" name="Nombre de la referencia" dataDxfId="39"/>
+    <tableColumn id="21" name="Nombre de la referencia para el proveedor" dataDxfId="38"/>
+    <tableColumn id="20" name="Descripción" dataDxfId="37"/>
+    <tableColumn id="19" name="Cantidad en Bodega Local" dataDxfId="36"/>
+    <tableColumn id="18" name="Cantidad en Zona Franca" dataDxfId="35"/>
+    <tableColumn id="17" name="Activo" dataDxfId="34"/>
+    <tableColumn id="26" name="Cantidad Minima para Alarma" dataDxfId="33"/>
+    <tableColumn id="27" name="Combinado" dataDxfId="32">
       <calculatedColumnFormula>IF(A6&lt;&gt;"",IF(B6&lt;&gt;"",CONCATENATE(A6,"-",B6),""),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3388,111 +3474,125 @@
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Tabla20212223242531" displayName="Tabla20212223242531" ref="A5:J6" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Tabla20212223242531" displayName="Tabla20212223242531" ref="A5:J6" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" tableBorderDxfId="29">
   <tableColumns count="10">
-    <tableColumn id="1" name="Tipo de Identificación" dataDxfId="19"/>
-    <tableColumn id="15" name="Identificación" dataDxfId="18"/>
-    <tableColumn id="22" name="Código" dataDxfId="17"/>
-    <tableColumn id="23" name="Nombre" dataDxfId="16"/>
-    <tableColumn id="20" name="Dirección" dataDxfId="15"/>
-    <tableColumn id="21" name="Teléfono" dataDxfId="14"/>
-    <tableColumn id="18" name="Fax" dataDxfId="13"/>
-    <tableColumn id="19" name="Correo Electrónico" dataDxfId="12" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="16" name="Contacto" dataDxfId="11"/>
-    <tableColumn id="17" name="Ciudad" dataDxfId="10"/>
+    <tableColumn id="1" name="Tipo de Identificación" dataDxfId="28"/>
+    <tableColumn id="15" name="Identificación" dataDxfId="27"/>
+    <tableColumn id="22" name="Código" dataDxfId="26"/>
+    <tableColumn id="23" name="Nombre" dataDxfId="25"/>
+    <tableColumn id="20" name="Dirección" dataDxfId="24"/>
+    <tableColumn id="21" name="Teléfono" dataDxfId="23"/>
+    <tableColumn id="18" name="Fax" dataDxfId="22"/>
+    <tableColumn id="19" name="Correo Electrónico" dataDxfId="21" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="16" name="Contacto" dataDxfId="20"/>
+    <tableColumn id="17" name="Ciudad" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Tabla20212223242532" displayName="Tabla20212223242532" ref="A5:B6" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="Tabla20212223242532" displayName="Tabla20212223242532" ref="A5:B6" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" tableBorderDxfId="16">
   <tableColumns count="2">
-    <tableColumn id="1" name="Código del Proveedor" dataDxfId="6"/>
-    <tableColumn id="15" name="Referencia" dataDxfId="5"/>
+    <tableColumn id="1" name="Código del Proveedor" dataDxfId="15"/>
+    <tableColumn id="15" name="Referencia" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla10" displayName="Tabla10" ref="A5:B7" totalsRowShown="0" headerRowDxfId="204" dataDxfId="203" tableBorderDxfId="202">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabla10" displayName="Tabla10" ref="A5:B7" totalsRowShown="0" headerRowDxfId="213" dataDxfId="212" tableBorderDxfId="211">
   <tableColumns count="2">
-    <tableColumn id="1" name="Actividad" dataDxfId="201"/>
-    <tableColumn id="2" name="Area" dataDxfId="200"/>
+    <tableColumn id="1" name="Actividad" dataDxfId="210"/>
+    <tableColumn id="2" name="Area" dataDxfId="209"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Tabla20212223242533" displayName="Tabla20212223242533" ref="A5:B9" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" tableBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="Tabla20212223242533" displayName="Tabla20212223242533" ref="A5:B9" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre del Método" dataDxfId="1"/>
-    <tableColumn id="15" name="Descripción" dataDxfId="0"/>
+    <tableColumn id="1" name="Nombre del Método" dataDxfId="10"/>
+    <tableColumn id="15" name="Descripción" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla202122232425332" displayName="Tabla202122232425332" ref="A5:F6" totalsRowShown="0" headerRowDxfId="6" dataDxfId="8" tableBorderDxfId="7">
+  <tableColumns count="6">
+    <tableColumn id="1" name="Referencia Interna artículo" dataDxfId="5"/>
+    <tableColumn id="15" name="Peso" dataDxfId="4"/>
+    <tableColumn id="2" name="Tamaño" dataDxfId="3"/>
+    <tableColumn id="3" name="Ancho" dataDxfId="2"/>
+    <tableColumn id="4" name="Alto" dataDxfId="0"/>
+    <tableColumn id="5" name="Cantidad" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla12" displayName="Tabla12" ref="A5:B9" totalsRowShown="0" headerRowDxfId="199" dataDxfId="198" tableBorderDxfId="197">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabla12" displayName="Tabla12" ref="A5:B9" totalsRowShown="0" headerRowDxfId="208" dataDxfId="207" tableBorderDxfId="206">
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre del Motivo" dataDxfId="196"/>
-    <tableColumn id="2" name="Descripción" dataDxfId="195"/>
+    <tableColumn id="1" name="Nombre del Motivo" dataDxfId="205"/>
+    <tableColumn id="2" name="Descripción" dataDxfId="204"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla13" displayName="Tabla13" ref="A5:B7" totalsRowShown="0" headerRowDxfId="194" dataDxfId="193" tableBorderDxfId="192">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Tabla13" displayName="Tabla13" ref="A5:B7" totalsRowShown="0" headerRowDxfId="203" dataDxfId="202" tableBorderDxfId="201">
   <tableColumns count="2">
-    <tableColumn id="1" name="Nombre del Tipo de Ajuste" dataDxfId="191"/>
-    <tableColumn id="2" name="Afectación sobre el Inventario" dataDxfId="190"/>
+    <tableColumn id="1" name="Nombre del Tipo de Ajuste" dataDxfId="200"/>
+    <tableColumn id="2" name="Afectación sobre el Inventario" dataDxfId="199"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla14" displayName="Tabla14" ref="A5:C8" totalsRowShown="0" headerRowDxfId="189" dataDxfId="188" tableBorderDxfId="187">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabla14" displayName="Tabla14" ref="A5:C8" totalsRowShown="0" headerRowDxfId="198" dataDxfId="197" tableBorderDxfId="196">
   <tableColumns count="3">
-    <tableColumn id="1" name="Tipo de Documento" dataDxfId="186"/>
-    <tableColumn id="2" name="Nombre del Tipo de Alarma" dataDxfId="185"/>
-    <tableColumn id="3" name="Descripcion" dataDxfId="184"/>
+    <tableColumn id="1" name="Tipo de Documento" dataDxfId="195"/>
+    <tableColumn id="2" name="Nombre del Tipo de Alarma" dataDxfId="194"/>
+    <tableColumn id="3" name="Descripcion" dataDxfId="193"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabla15" displayName="Tabla15" ref="A5:B7" totalsRowShown="0" headerRowDxfId="183" dataDxfId="182" tableBorderDxfId="181">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Tabla15" displayName="Tabla15" ref="A5:B7" totalsRowShown="0" headerRowDxfId="192" dataDxfId="191" tableBorderDxfId="190">
   <tableColumns count="2">
-    <tableColumn id="1" name="Tipo de Alarma" dataDxfId="180"/>
-    <tableColumn id="2" name="Mensaje" dataDxfId="179"/>
+    <tableColumn id="1" name="Tipo de Alarma" dataDxfId="189"/>
+    <tableColumn id="2" name="Mensaje" dataDxfId="188"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla16" displayName="Tabla16" ref="A5:C8" totalsRowShown="0" headerRowDxfId="178" dataDxfId="177" tableBorderDxfId="176">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Tabla16" displayName="Tabla16" ref="A5:C8" totalsRowShown="0" headerRowDxfId="187" dataDxfId="186" tableBorderDxfId="185">
   <tableColumns count="3">
-    <tableColumn id="1" name="Nombre del Motivo" dataDxfId="175"/>
-    <tableColumn id="2" name="Tipo de Documento" dataDxfId="174"/>
-    <tableColumn id="3" name="Descripción" dataDxfId="173"/>
+    <tableColumn id="1" name="Nombre del Motivo" dataDxfId="184"/>
+    <tableColumn id="2" name="Tipo de Documento" dataDxfId="183"/>
+    <tableColumn id="3" name="Descripción" dataDxfId="182"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tabla18" displayName="Tabla18" ref="A5:C8" totalsRowShown="0" headerRowDxfId="172" dataDxfId="171" tableBorderDxfId="170">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tabla18" displayName="Tabla18" ref="A5:C8" totalsRowShown="0" headerRowDxfId="181" dataDxfId="180" tableBorderDxfId="179">
   <tableColumns count="3">
-    <tableColumn id="1" name="Nombre del Motivo" dataDxfId="169"/>
-    <tableColumn id="2" name="Tipo de Documento" dataDxfId="168"/>
-    <tableColumn id="3" name="Descripción" dataDxfId="167"/>
+    <tableColumn id="1" name="Nombre del Motivo" dataDxfId="178"/>
+    <tableColumn id="2" name="Tipo de Documento" dataDxfId="177"/>
+    <tableColumn id="3" name="Descripción" dataDxfId="176"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3812,96 +3912,96 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="63"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="65"/>
     </row>
     <row r="2" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="59"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="61"/>
     </row>
     <row r="3" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="61"/>
     </row>
     <row r="4" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="59"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="61"/>
     </row>
     <row r="6" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="59"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="61"/>
     </row>
     <row r="7" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -3972,58 +4072,58 @@
       <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
-      <c r="H10" s="58"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="58"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="58"/>
-      <c r="M10" s="59"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="61"/>
     </row>
     <row r="11" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
-      <c r="J11" s="58"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="58"/>
-      <c r="M11" s="59"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="61"/>
     </row>
     <row r="12" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="61"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4151,7 +4251,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,"@IDDOCUMENT",$X$2,IF(LEN(C6)&gt;0,CONCATENATE($W$2,C6,$W$2),$Z$2))</f>
         <v>'Error en cantidades',@IDDOCUMENT,NULL</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDDOCUMENT SMALLINT = (SELECT DOCUMENT_TYPE_ID FROM document_types WHERE DOCUMENT_TYPE_NAME = 'Pedido') insert into modification_reasons (MODIFICATION_REASON_NAME, DOCUMENT_TYPE_ID, NOTES) values  ('Error en cantidades',@IDDOCUMENT,NULL)
 GO</v>
@@ -4175,7 +4275,7 @@
         <f t="shared" ref="R7:R8" si="1">CONCATENATE($W$2,A7,$W$2,$X$2,"@IDDOCUMENT",$X$2,IF(LEN(C7)&gt;0,CONCATENATE($W$2,C7,$W$2),$Z$2))</f>
         <v>'Eliminar Articulos',@IDDOCUMENT,NULL</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7:T8" si="2">CONCATENATE(P7," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDDOCUMENT SMALLINT = (SELECT DOCUMENT_TYPE_ID FROM document_types WHERE DOCUMENT_TYPE_NAME = 'Orden') insert into modification_reasons (MODIFICATION_REASON_NAME, DOCUMENT_TYPE_ID, NOTES) values  ('Eliminar Articulos',@IDDOCUMENT,NULL)
 GO</v>
@@ -4199,7 +4299,7 @@
         <f t="shared" si="1"/>
         <v>'Cambio de vencimiento',@IDDOCUMENT,NULL</v>
       </c>
-      <c r="T8" s="67" t="str">
+      <c r="T8" s="59" t="str">
         <f t="shared" si="2"/>
         <v>DECLARE @IDDOCUMENT SMALLINT = (SELECT DOCUMENT_TYPE_ID FROM document_types WHERE DOCUMENT_TYPE_NAME = 'Reserva') insert into modification_reasons (MODIFICATION_REASON_NAME, DOCUMENT_TYPE_ID, NOTES) values  ('Cambio de vencimiento',@IDDOCUMENT,NULL)
 GO</v>
@@ -4317,7 +4417,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,IF(LEN(C6)&gt;0,CONCATENATE($W$2,C6,$W$2),$Z$2))</f>
         <v>'Falta de Articulos',NULL</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2)</f>
         <v>insert into close_customer_order_reasons (CLOSE_REASON_NAME, CLOSE_REASON_NOTES) values  ('Falta de Articulos',NULL)</v>
       </c>
@@ -4330,7 +4430,7 @@
         <f t="shared" ref="R7:R8" si="0">CONCATENATE($W$2,A7,$W$2,$X$2,IF(LEN(C7)&gt;0,CONCATENATE($W$2,C7,$W$2),$Z$2))</f>
         <v>'Solicitud del Cliente',NULL</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7:T8" si="1">CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2)</f>
         <v>insert into close_customer_order_reasons (CLOSE_REASON_NAME, CLOSE_REASON_NOTES) values  ('Solicitud del Cliente',NULL)</v>
       </c>
@@ -4343,14 +4443,14 @@
         <f t="shared" si="0"/>
         <v>'Error en Pedido',NULL</v>
       </c>
-      <c r="T8" s="67" t="str">
+      <c r="T8" s="59" t="str">
         <f t="shared" si="1"/>
         <v>insert into close_customer_order_reasons (CLOSE_REASON_NAME, CLOSE_REASON_NOTES) values  ('Error en Pedido',NULL)</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="R9" s="53"/>
-      <c r="T9" s="67"/>
+      <c r="T9" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4461,7 +4561,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,$W$2,B6,$W$2)</f>
         <v>'Colombia','CO'</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2)</f>
         <v>insert into countries (COUNTRY_NAME, COUNTRY_CODE) values  ('Colombia','CO')</v>
       </c>
@@ -4477,14 +4577,14 @@
         <f>CONCATENATE($W$2,A7,$W$2,$X$2,$W$2,B7,$W$2)</f>
         <v>'Estados Unidos','USA'</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7" si="0">CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2)</f>
         <v>insert into countries (COUNTRY_NAME, COUNTRY_CODE) values  ('Estados Unidos','USA')</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="R8" s="53"/>
-      <c r="T8" s="67"/>
+      <c r="T8" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4616,7 +4716,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,"@IDCOUNTRY")</f>
         <v>'Cundinamarca',@IDCOUNTRY</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDCOUNTRY INT = (SELECT COUNTRY_ID FROM countries WHERE COUNTRY_CODE = 'CO') insert into departments (DEPARTMENT_NAME, COUNTRY_ID) values  ('Cundinamarca',@IDCOUNTRY)
 GO</v>
@@ -4641,7 +4741,7 @@
         <f t="shared" ref="R7:R8" si="1">CONCATENATE($W$2,A7,$W$2,$X$2,"@IDCOUNTRY")</f>
         <v>'Antioquia',@IDCOUNTRY</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7:T8" si="2">CONCATENATE(P7," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDCOUNTRY INT = (SELECT COUNTRY_ID FROM countries WHERE COUNTRY_CODE = 'CO') insert into departments (DEPARTMENT_NAME, COUNTRY_ID) values  ('Antioquia',@IDCOUNTRY)
 GO</v>
@@ -4666,7 +4766,7 @@
         <f t="shared" si="1"/>
         <v>'Florida',@IDCOUNTRY</v>
       </c>
-      <c r="T8" s="67" t="str">
+      <c r="T8" s="59" t="str">
         <f t="shared" si="2"/>
         <v>DECLARE @IDCOUNTRY INT = (SELECT COUNTRY_ID FROM countries WHERE COUNTRY_CODE = 'USA') insert into departments (DEPARTMENT_NAME, COUNTRY_ID) values  ('Florida',@IDCOUNTRY)
 GO</v>
@@ -4803,7 +4903,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,"@IDDEPARTAMENT")</f>
         <v>'Bogota',@IDDEPARTAMENT</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDDEPARTAMENT INT = (SELECT DEPARTMENT_ID from departments a join countries b ON b.COUNTRY_ID = a.COUNTRY_ID WHERE B.COUNTRY_CODE+'-'+A.DEPARTMENT_NAME = 'CO-Cundinamarca') insert into cities (CITY_NAME, DEPARTMENT_ID) values  ('Bogota',@IDDEPARTAMENT)
 GO</v>
@@ -4828,7 +4928,7 @@
         <f t="shared" ref="R7:R8" si="1">CONCATENATE($W$2,A7,$W$2,$X$2,"@IDDEPARTAMENT")</f>
         <v>'Chia',@IDDEPARTAMENT</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7:T8" si="2">CONCATENATE(P7," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDDEPARTAMENT INT = (SELECT DEPARTMENT_ID from departments a join countries b ON b.COUNTRY_ID = a.COUNTRY_ID WHERE B.COUNTRY_CODE+'-'+A.DEPARTMENT_NAME = 'CO-Cundinamarca') insert into cities (CITY_NAME, DEPARTMENT_ID) values  ('Chia',@IDDEPARTAMENT)
 GO</v>
@@ -4853,7 +4953,7 @@
         <f t="shared" si="1"/>
         <v>'Miami',@IDDEPARTAMENT</v>
       </c>
-      <c r="T8" s="67" t="str">
+      <c r="T8" s="59" t="str">
         <f t="shared" si="2"/>
         <v>DECLARE @IDDEPARTAMENT INT = (SELECT DEPARTMENT_ID from departments a join countries b ON b.COUNTRY_ID = a.COUNTRY_ID WHERE B.COUNTRY_CODE+'-'+A.DEPARTMENT_NAME = 'USA-Florida') insert into cities (CITY_NAME, DEPARTMENT_ID) values  ('Miami',@IDDEPARTAMENT)
 GO</v>
@@ -4975,7 +5075,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,$W$2,B6,$W$2)</f>
         <v>'CC','Cédula de Ciudadania'</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2)</f>
         <v>insert into identity_types (IDENTITY_TYPE_CODE, IDENTITY_TYPE_NAME) values  ('CC','Cédula de Ciudadania')</v>
       </c>
@@ -4991,7 +5091,7 @@
         <f>CONCATENATE($W$2,A7,$W$2,$X$2,$W$2,B7,$W$2)</f>
         <v>'NIT','Nit Empresa'</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7" si="0">CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2)</f>
         <v>insert into identity_types (IDENTITY_TYPE_CODE, IDENTITY_TYPE_NAME) values  ('NIT','Nit Empresa')</v>
       </c>
@@ -5238,7 +5338,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,$W$2,B6,$W$2,$X$2,"@IDIDENTTYPE",$X$2,$W$2,D6,$W$2,$X$2,$W$2,E6,$W$2,$X$2,IF(LEN(F6)&gt;0,CONCATENATE($W$2,F6,$W$2),$Z$2),$X$2,IF(LEN(G6)&gt;0,CONCATENATE($W$2,G6,$W$2),$Z$2),$X$2,"@IDCITY",$X$2,$W$2,I6,$W$2,$X$2,"@ISACTIVE")</f>
         <v>'Satelite Mugs','Proplasticos',@IDIDENTTYPE,'123458','3007854516',NULL,'mugs@gmail.com',@IDCITY,'Fulanito',@ISACTIVE</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(O6," ",Q6," ",P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDIDENTTYPE INT = (SELECT IDENTITY_TYPE_ID FROM identity_types WHERE IDENTITY_TYPE_CODE =  'NIT') DECLARE @ISACTIVE BIT = (CASE WHEN 'Si' = 'Si' THEN 1 ELSE 0 END) DECLARE @IDCITY INT = (SELECT CITY_ID FROM cities a JOIN departments b ON b.DEPARTMENT_ID = a.DEPARTMENT_ID JOIN countries c ON c.COUNTRY_ID = B.COUNTRY_ID WHERE c.COUNTRY_CODE +'-'+B.DEPARTMENT_NAME+'-'+a.CITY_NAME = 'USA-Florida-Miami') insert into process_satellites (PROCESS_SATELLITE_NAME, PROCESS_SATELLITE_ADDRESS, IDENTITY_TYPE_ID, IDENTITY_NUMBER, PHONE, FAX, EMAIL, CITY_ID, LEGAL_REPRESENTATIVE, IS_ACTIVE) values  ('Satelite Mugs','Proplasticos',@IDIDENTTYPE,'123458','3007854516',NULL,'mugs@gmail.com',@IDCITY,'Fulanito',@ISACTIVE)
 GO</v>
@@ -5291,7 +5391,7 @@
         <f t="shared" ref="R7:R8" si="3">CONCATENATE($W$2,A7,$W$2,$X$2,$W$2,B7,$W$2,$X$2,"@IDIDENTTYPE",$X$2,$W$2,D7,$W$2,$X$2,$W$2,E7,$W$2,$X$2,IF(LEN(F7)&gt;0,CONCATENATE($W$2,F7,$W$2),$Z$2),$X$2,IF(LEN(G7)&gt;0,CONCATENATE($W$2,G7,$W$2),$Z$2),$X$2,"@IDCITY",$X$2,$W$2,I7,$W$2,$X$2,"@ISACTIVE")</f>
         <v>'Planta','Proplasticos',@IDIDENTTYPE,'568745','3016254578',NULL,'planta@catalogospromocionales.com',@IDCITY,'Gustavo Ramirez',@ISACTIVE</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7:T8" si="4">CONCATENATE(O7," ",Q7," ",P7," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDIDENTTYPE INT = (SELECT IDENTITY_TYPE_ID FROM identity_types WHERE IDENTITY_TYPE_CODE =  'NIT') DECLARE @ISACTIVE BIT = (CASE WHEN 'Si' = 'Si' THEN 1 ELSE 0 END) DECLARE @IDCITY INT = (SELECT CITY_ID FROM cities a JOIN departments b ON b.DEPARTMENT_ID = a.DEPARTMENT_ID JOIN countries c ON c.COUNTRY_ID = B.COUNTRY_ID WHERE c.COUNTRY_CODE +'-'+B.DEPARTMENT_NAME+'-'+a.CITY_NAME = 'CO-Cundinamarca-Chia') insert into process_satellites (PROCESS_SATELLITE_NAME, PROCESS_SATELLITE_ADDRESS, IDENTITY_TYPE_ID, IDENTITY_NUMBER, PHONE, FAX, EMAIL, CITY_ID, LEGAL_REPRESENTATIVE, IS_ACTIVE) values  ('Planta','Proplasticos',@IDIDENTTYPE,'568745','3016254578',NULL,'planta@catalogospromocionales.com',@IDCITY,'Gustavo Ramirez',@ISACTIVE)
 GO</v>
@@ -5341,7 +5441,7 @@
         <f t="shared" si="3"/>
         <v>'Etipress S.A','Cra 39 B nº 17-98',@IDIDENTTYPE,'23658','3142458963',NULL,'etipress_info@etipress.com.co',@IDCITY,'Perencejo',@ISACTIVE</v>
       </c>
-      <c r="T8" s="67" t="str">
+      <c r="T8" s="59" t="str">
         <f t="shared" si="4"/>
         <v>DECLARE @IDIDENTTYPE INT = (SELECT IDENTITY_TYPE_ID FROM identity_types WHERE IDENTITY_TYPE_CODE =  'CC') DECLARE @ISACTIVE BIT = (CASE WHEN 'No' = 'Si' THEN 1 ELSE 0 END) DECLARE @IDCITY INT = (SELECT CITY_ID FROM cities a JOIN departments b ON b.DEPARTMENT_ID = a.DEPARTMENT_ID JOIN countries c ON c.COUNTRY_ID = B.COUNTRY_ID WHERE c.COUNTRY_CODE +'-'+B.DEPARTMENT_NAME+'-'+a.CITY_NAME = 'CO-Cundinamarca-Bogota') insert into process_satellites (PROCESS_SATELLITE_NAME, PROCESS_SATELLITE_ADDRESS, IDENTITY_TYPE_ID, IDENTITY_NUMBER, PHONE, FAX, EMAIL, CITY_ID, LEGAL_REPRESENTATIVE, IS_ACTIVE) values  ('Etipress S.A','Cra 39 B nº 17-98',@IDIDENTTYPE,'23658','3142458963',NULL,'etipress_info@etipress.com.co',@IDCITY,'Perencejo',@ISACTIVE)
 GO</v>
@@ -5641,7 +5741,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,$W$2,B6,$W$2,$X$2,"@IDIDENTTYPE",$X$2,$W$2,D6,$W$2,$X$2,$W$2,E6,$W$2,$X$2,IF(LEN(F6)&gt;0,CONCATENATE($W$2,F6,$W$2),$Z$2),$X$2,IF(LEN(G6)&gt;0,CONCATENATE($W$2,G6,$W$2),$Z$2),$X$2,"@IDCITY",$X$2,$W$2,I6,$W$2,$X$2,"@ISACTIVE")</f>
         <v>'CC','79872389',@IDIDENTTYPE,'3008987553','3004587458',NULL,'calle 4a # 29 - 25',@IDCITY,'ardc2440@gmail.com;paolaflorezp@gmail.com',@ISACTIVE</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(O6," ",Q6," ",P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDIDENTTYPE INT = (SELECT IDENTITY_TYPE_ID FROM identity_types WHERE IDENTITY_TYPE_CODE =  'Andres Diaz') DECLARE @ISACTIVE BIT = (CASE WHEN 'CO-Cundinamarca-Bogota' = 'Si' THEN 1 ELSE 0 END) DECLARE @IDCITY INT = (SELECT CITY_ID FROM cities a JOIN departments b ON b.DEPARTMENT_ID = a.DEPARTMENT_ID JOIN countries c ON c.COUNTRY_ID = B.COUNTRY_ID WHERE c.COUNTRY_CODE +'-'+B.DEPARTMENT_NAME+'-'+a.CITY_NAME = '3008987553') insert into customers (IDENTITY_TYPE_ID, IDENTITY_NUMBER, CUSTOMER_NAME, PHONE1, PHONE2, FAX, CUSTOMER_ADDRESS, CELL_PHONE, EMAIL, CITY_ID, SEND_EMAIL) values  ('CC','79872389',@IDIDENTTYPE,'3008987553','3004587458',NULL,'calle 4a # 29 - 25',@IDCITY,'ardc2440@gmail.com;paolaflorezp@gmail.com',@ISACTIVE)
 GO</v>
@@ -5701,7 +5801,7 @@
         <f t="shared" ref="R7" si="3">CONCATENATE($W$2,A7,$W$2,$X$2,$W$2,B7,$W$2,$X$2,"@IDIDENTTYPE",$X$2,$W$2,D7,$W$2,$X$2,$W$2,E7,$W$2,$X$2,IF(LEN(F7)&gt;0,CONCATENATE($W$2,F7,$W$2),$Z$2),$X$2,IF(LEN(G7)&gt;0,CONCATENATE($W$2,G7,$W$2),$Z$2),$X$2,"@IDCITY",$X$2,$W$2,I7,$W$2,$X$2,"@ISACTIVE")</f>
         <v>'CC','35427339',@IDIDENTTYPE,'3542658925','3112457856',NULL,'Carrera 2 b # 11 - 25',@IDCITY,'paolaflorezp@gmail.com',@ISACTIVE</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7" si="4">CONCATENATE(O7," ",Q7," ",P7," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDIDENTTYPE INT = (SELECT IDENTITY_TYPE_ID FROM identity_types WHERE IDENTITY_TYPE_CODE =  'Paola Florez') DECLARE @ISACTIVE BIT = (CASE WHEN 'CO-Cundinamarca-Chia' = 'Si' THEN 1 ELSE 0 END) DECLARE @IDCITY INT = (SELECT CITY_ID FROM cities a JOIN departments b ON b.DEPARTMENT_ID = a.DEPARTMENT_ID JOIN countries c ON c.COUNTRY_ID = B.COUNTRY_ID WHERE c.COUNTRY_CODE +'-'+B.DEPARTMENT_NAME+'-'+a.CITY_NAME = '3014296649') insert into customers (IDENTITY_TYPE_ID, IDENTITY_NUMBER, CUSTOMER_NAME, PHONE1, PHONE2, FAX, CUSTOMER_ADDRESS, CELL_PHONE, EMAIL, CITY_ID, SEND_EMAIL) values  ('CC','35427339',@IDIDENTTYPE,'3542658925','3112457856',NULL,'Carrera 2 b # 11 - 25',@IDCITY,'paolaflorezp@gmail.com',@ISACTIVE)
 GO</v>
@@ -5712,7 +5812,7 @@
       <c r="P8" s="53"/>
       <c r="Q8" s="53"/>
       <c r="R8" s="53"/>
-      <c r="T8" s="67"/>
+      <c r="T8" s="59"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5896,7 +5996,7 @@
         <f>CONCATENATE("@IDCUSTOMER",$X$2,$W$2,B6,$W$2,$X$2,$W$2,C6,$W$2,$X$2,$W$2,D6,$W$2,$X$2,IF(LEN(E6)&gt;0,CONCATENATE($W$2,E6,$W$2),$Z$2))</f>
         <v>@IDCUSTOMER,'andres diaz','propietario','3008987553','ardc2440@gmail.com'</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDCUSTOMER INT = (SELECT CITY_ID FROM customers a JOIN identity_types b ON b.IDENTITY_TYPE_ID = a.IDENTITY_TYPE_ID WHERE b.IDENTITY_TYPE_CODE +'-'+a.IDENTITY_NUMBER = 'CC-79872389') insert into customer_contacts (CUSTOMER_ID, CUSTOMER_CONTACT_NAME, TITLE, PHONE, EMAIL) values  (@IDCUSTOMER,'andres diaz','propietario','3008987553','ardc2440@gmail.com')
 GO</v>
@@ -5927,7 +6027,7 @@
         <f>CONCATENATE("@IDCUSTOMER",$X$2,$W$2,B7,$W$2,$X$2,$W$2,C7,$W$2,$X$2,$W$2,D7,$W$2,$X$2,IF(LEN(E7)&gt;0,CONCATENATE($W$2,E7,$W$2),$Z$2))</f>
         <v>@IDCUSTOMER,'Paola Florez','Gerente','3014662769','paolaflorezp@gmail.com'</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f>CONCATENATE(P7," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDCUSTOMER INT = (SELECT CITY_ID FROM customers a JOIN identity_types b ON b.IDENTITY_TYPE_ID = a.IDENTITY_TYPE_ID WHERE b.IDENTITY_TYPE_CODE +'-'+a.IDENTITY_NUMBER = 'CC-35427339') insert into customer_contacts (CUSTOMER_ID, CUSTOMER_CONTACT_NAME, TITLE, PHONE, EMAIL) values  (@IDCUSTOMER,'Paola Florez','Gerente','3014662769','paolaflorezp@gmail.com')
 GO</v>
@@ -6134,7 +6234,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,$W$2,B6,$W$2,$X$2,IF(LEN(C6)&gt;0,CONCATENATE($W$2,C6,$W$2),$Z$2),$X$2,IF(LEN(D6)&gt;0,CONCATENATE($W$2,D6,$W$2),$Z$2),$X$2,$W$2,E6,$W$2,$X$2,IF(LEN(F6)&gt;0,CONCATENATE($W$2,F6,$W$2),$Z$2),$X$2,IF(LEN(G6)&gt;0,CONCATENATE($W$2,G6,$W$2),$Z$2),$X$2,"@IDCITY")</f>
         <v>'trasportes fusa','745585','22222','5456456452','calle 15 parque internacional central','InterTransMar@gmail.com',NULL,@IDCITY</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDCITY INT = (SELECT CITY_ID FROM cities a JOIN departments b ON b.DEPARTMENT_ID = a.DEPARTMENT_ID JOIN countries c ON c.COUNTRY_ID = B.COUNTRY_ID WHERE c.COUNTRY_CODE +'-'+B.DEPARTMENT_NAME+'-'+a.CITY_NAME = 'CO-Cundinamarca-Chia') insert into forwarders (FORWARDER_NAME, PHONE1, PHONE2, FAX, FORWARDER_ADDRESS, MAIL1, MAIL2, CITY_ID) values  ('trasportes fusa','745585','22222','5456456452','calle 15 parque internacional central','InterTransMar@gmail.com',NULL,@IDCITY)
 GO</v>
@@ -6165,7 +6265,7 @@
         <f>CONCATENATE($W$2,A7,$W$2,$X$2,$W$2,B7,$W$2,$X$2,IF(LEN(C7)&gt;0,CONCATENATE($W$2,C7,$W$2),$Z$2),$X$2,IF(LEN(D7)&gt;0,CONCATENATE($W$2,D7,$W$2),$Z$2),$X$2,$W$2,E7,$W$2,$X$2,IF(LEN(F7)&gt;0,CONCATENATE($W$2,F7,$W$2),$Z$2),$X$2,IF(LEN(G7)&gt;0,CONCATENATE($W$2,G7,$W$2),$Z$2),$X$2,"@IDCITY")</f>
         <v>'International Trans Mar','745585',NULL,NULL,'la casona local 1234',NULL,'mi_correo@correo.com',@IDCITY</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f>CONCATENATE(P7," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDCITY INT = (SELECT CITY_ID FROM cities a JOIN departments b ON b.DEPARTMENT_ID = a.DEPARTMENT_ID JOIN countries c ON c.COUNTRY_ID = B.COUNTRY_ID WHERE c.COUNTRY_CODE +'-'+B.DEPARTMENT_NAME+'-'+a.CITY_NAME = 'USA-Florida-Miami') insert into forwarders (FORWARDER_NAME, PHONE1, PHONE2, FAX, FORWARDER_ADDRESS, MAIL1, MAIL2, CITY_ID) values  ('International Trans Mar','745585',NULL,NULL,'la casona local 1234',NULL,'mi_correo@correo.com',@IDCITY)
 GO</v>
@@ -6276,7 +6376,7 @@
         <f>CONCATENATE($W$2,A6,$W$2)</f>
         <v>'Logo Pendiente'</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2)</f>
         <v>insert into activity_types (ACTIVITY_TYPE_NAME) values  ('Logo Pendiente')</v>
       </c>
@@ -6289,7 +6389,7 @@
         <f>CONCATENATE($W$2,A7,$W$2)</f>
         <v>'Pedido Incompleto'</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f>CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2)</f>
         <v>insert into activity_types (ACTIVITY_TYPE_NAME) values  ('Pedido Incompleto')</v>
       </c>
@@ -6517,7 +6617,7 @@
         <f>CONCATENATE("@IDFORWARDER",$X$2,$W$2,B6,$W$2,$X$2,$W$2,C6,$W$2,$X$2,IF(LEN(D6)&gt;0,CONCATENATE($W$2,D6,$W$2),$Z$2),$X$2,IF(LEN(E6)&gt;0,CONCATENATE($W$2,E6,$W$2),$Z$2),$X$2,$W$2,F6,$W$2,$X$2,"@IDCITY",$X$2,$W$2,H6,$W$2,$X$2,IF(LEN(I6)&gt;0,CONCATENATE($W$2,I6,$W$2),$Z$2),$X$2,IF(LEN(J6)&gt;0,CONCATENATE($W$2,J6,$W$2),$Z$2))</f>
         <v>@IDFORWARDER,'Carmelita la nita','5454548787','21352124',NULL,'Calle 40 # 20 - 23',@IDCITY,'Camela Nita Lopez','carmela@fusa.com',NULL</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(N6," ",P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDFORWARDER INT = (SELECT FORWARDER_ID FROM forwarders WHERE FORWARDER_NAME = 'trasportes fusa') DECLARE @IDCITY INT = (SELECT CITY_ID FROM cities a JOIN departments b ON b.DEPARTMENT_ID = a.DEPARTMENT_ID JOIN countries c ON c.COUNTRY_ID = B.COUNTRY_ID WHERE c.COUNTRY_CODE +'-'+B.DEPARTMENT_NAME+'-'+a.CITY_NAME = 'CO-Cundinamarca-Bogota') insert into forwarder_agents (FORWARDER_ID, FORWARDER_AGENT_NAME, PHONE1, PHONE2, FAX, FORWARDER_AGENT_ADDRESS, CITY_ID, CONTACT, EMAIL1, EMAIL2) values  (@IDFORWARDER,'Carmelita la nita','5454548787','21352124',NULL,'Calle 40 # 20 - 23',@IDCITY,'Camela Nita Lopez','carmela@fusa.com',NULL)
 GO</v>
@@ -6566,7 +6666,7 @@
         <f>CONCATENATE("@IDFORWARDER",$X$2,$W$2,B7,$W$2,$X$2,$W$2,C7,$W$2,$X$2,IF(LEN(D7)&gt;0,CONCATENATE($W$2,D7,$W$2),$Z$2),$X$2,IF(LEN(E7)&gt;0,CONCATENATE($W$2,E7,$W$2),$Z$2),$X$2,$W$2,F7,$W$2,$X$2,"@IDCITY",$X$2,$W$2,H7,$W$2,$X$2,IF(LEN(I7)&gt;0,CONCATENATE($W$2,I7,$W$2),$Z$2),$X$2,IF(LEN(J7)&gt;0,CONCATENATE($W$2,J7,$W$2),$Z$2))</f>
         <v>@IDFORWARDER,'Transmar Colombia','54252262','875412363',NULL,'Calle 28 # 12 - 35',@IDCITY,'Jose Lopez',NULL,'Lopez.jose@transmar.com'</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f>CONCATENATE(N7," ",P7," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDFORWARDER INT = (SELECT FORWARDER_ID FROM forwarders WHERE FORWARDER_NAME = 'International Trans Mar') DECLARE @IDCITY INT = (SELECT CITY_ID FROM cities a JOIN departments b ON b.DEPARTMENT_ID = a.DEPARTMENT_ID JOIN countries c ON c.COUNTRY_ID = B.COUNTRY_ID WHERE c.COUNTRY_CODE +'-'+B.DEPARTMENT_NAME+'-'+a.CITY_NAME = 'CO-Cundinamarca-Chia') insert into forwarder_agents (FORWARDER_ID, FORWARDER_AGENT_NAME, PHONE1, PHONE2, FAX, FORWARDER_AGENT_ADDRESS, CITY_ID, CONTACT, EMAIL1, EMAIL2) values  (@IDFORWARDER,'Transmar Colombia','54252262','875412363',NULL,'Calle 28 # 12 - 35',@IDCITY,'Jose Lopez',NULL,'Lopez.jose@transmar.com')
 GO</v>
@@ -6696,7 +6796,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,$W$2,B6,$W$2)</f>
         <v>'Aereo','Transporte Aéreo'</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2)</f>
         <v>insert into shipment_methods (SHIPMENT_METHOD_NAME, SHIPMENT_METHOD_NOTES) values  ('Aereo','Transporte Aéreo')</v>
       </c>
@@ -6712,7 +6812,7 @@
         <f t="shared" ref="R7:R9" si="0">CONCATENATE($W$2,A7,$W$2,$X$2,$W$2,B7,$W$2)</f>
         <v>'Maritimo','Transporte Marítimo'</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7:T9" si="1">CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2)</f>
         <v>insert into shipment_methods (SHIPMENT_METHOD_NAME, SHIPMENT_METHOD_NOTES) values  ('Maritimo','Transporte Marítimo')</v>
       </c>
@@ -6728,7 +6828,7 @@
         <f t="shared" si="0"/>
         <v>'Combinado','Transporte Aéreo y Marítimo'</v>
       </c>
-      <c r="T8" s="67" t="str">
+      <c r="T8" s="59" t="str">
         <f t="shared" si="1"/>
         <v>insert into shipment_methods (SHIPMENT_METHOD_NAME, SHIPMENT_METHOD_NOTES) values  ('Combinado','Transporte Aéreo y Marítimo')</v>
       </c>
@@ -6744,7 +6844,7 @@
         <f t="shared" si="0"/>
         <v>'Directo','Entrega local'</v>
       </c>
-      <c r="T9" s="67" t="str">
+      <c r="T9" s="59" t="str">
         <f t="shared" si="1"/>
         <v>insert into shipment_methods (SHIPMENT_METHOD_NAME, SHIPMENT_METHOD_NOTES) values  ('Directo','Entrega local')</v>
       </c>
@@ -6861,7 +6961,7 @@
         <f>CONCATENATE("@SHIPMENTMETHODID",$X$2,"@FORWARDERAGENTID")</f>
         <v>@SHIPMENTMETHODID,@FORWARDERAGENTID</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(N6," ",P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @SHIPMENTMETHODID INT = (SELECT SHIPMENT_METHOD_ID FROM shipment_methods WHERE SHIPMENT_METHOD_NAME = 'Aereo') DECLARE @FORWARDERAGENTID INT = (SELECT FORWARDER_AGENT_ID FROM forwarder_agents a JOIN forwarders b ON b.FORWARDER_ID = a.FORWARDER_ID WHERE b.FORWARDER_NAME +'-'+a.FORWARDER_AGENT_NAME = 'trasportes fusa-Carmelita la nita') insert into shipment_forwarder_agent_methods (SHIPMENT_METHOD_ID, FORWARDER_AGENT_ID) values  (@SHIPMENTMETHODID,@FORWARDERAGENTID)
 GO</v>
@@ -6887,7 +6987,7 @@
         <f>CONCATENATE("@SHIPMENTMETHODID",$X$2,"@FORWARDERAGENTID")</f>
         <v>@SHIPMENTMETHODID,@FORWARDERAGENTID</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f>CONCATENATE(N7," ",P7," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @SHIPMENTMETHODID INT = (SELECT SHIPMENT_METHOD_ID FROM shipment_methods WHERE SHIPMENT_METHOD_NAME = 'Maritimo') DECLARE @FORWARDERAGENTID INT = (SELECT FORWARDER_AGENT_ID FROM forwarder_agents a JOIN forwarders b ON b.FORWARDER_ID = a.FORWARDER_ID WHERE b.FORWARDER_NAME +'-'+a.FORWARDER_AGENT_NAME = 'International Trans Mar-Transmar Colombia') insert into shipment_forwarder_agent_methods (SHIPMENT_METHOD_ID, FORWARDER_AGENT_ID) values  (@SHIPMENTMETHODID,@FORWARDERAGENTID)
 GO</v>
@@ -7053,7 +7153,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,$W$2,B6,$W$2,$X$2,"@ISDEMON",$X$2,"@ISACTIVE")</f>
         <v>'001','Importados',@ISDEMON,@ISACTIVE</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(N6," ",P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @ISDEMON BIT = (CASE WHEN 'Si' = 'Si' THEN 1 ELSE 0 END) DECLARE @ISACTIVE BIT = (CASE WHEN 'Si' = 'Si' THEN 1 ELSE 0 END) insert into lines (LINE_CODE, LINE_NAME, IS_DEMON, IS_ACTIVE) values  ('001','Importados',@ISDEMON,@ISACTIVE)
 GO</v>
@@ -7154,7 +7254,7 @@
         <f>CONCATENATE($W$2,A6,$W$2)</f>
         <v>'EURO'</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2)</f>
         <v>insert into currencies (CURRENCY_NAME) values  ('EURO')</v>
       </c>
@@ -7167,7 +7267,7 @@
         <f t="shared" ref="R7:R8" si="0">CONCATENATE($W$2,A7,$W$2)</f>
         <v>'PESO'</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7:T8" si="1">CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2)</f>
         <v>insert into currencies (CURRENCY_NAME) values  ('PESO')</v>
       </c>
@@ -7180,7 +7280,7 @@
         <f t="shared" si="0"/>
         <v>'USD'</v>
       </c>
-      <c r="T8" s="67" t="str">
+      <c r="T8" s="59" t="str">
         <f t="shared" si="1"/>
         <v>insert into currencies (CURRENCY_NAME) values  ('USD')</v>
       </c>
@@ -7273,7 +7373,7 @@
         <f>CONCATENATE($W$2,A6,$W$2)</f>
         <v>'Caja'</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2)</f>
         <v>insert into measure_units (MEASURE_UNIT_NAME) values  ('Caja')</v>
       </c>
@@ -7286,7 +7386,7 @@
         <f t="shared" ref="R7:R8" si="0">CONCATENATE($W$2,A7,$W$2)</f>
         <v>'Centimetro Cúbico'</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7:T8" si="1">CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2)</f>
         <v>insert into measure_units (MEASURE_UNIT_NAME) values  ('Centimetro Cúbico')</v>
       </c>
@@ -7299,7 +7399,7 @@
         <f t="shared" si="0"/>
         <v>'Gramo'</v>
       </c>
-      <c r="T8" s="67" t="str">
+      <c r="T8" s="59" t="str">
         <f t="shared" si="1"/>
         <v>insert into measure_units (MEASURE_UNIT_NAME) values  ('Gramo')</v>
       </c>
@@ -7312,7 +7412,7 @@
         <f t="shared" ref="R9" si="2">CONCATENATE($W$2,A9,$W$2)</f>
         <v>'Pieza'</v>
       </c>
-      <c r="T9" s="67" t="str">
+      <c r="T9" s="59" t="str">
         <f t="shared" ref="T9" si="3">CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R9,$Y$2)</f>
         <v>insert into measure_units (MEASURE_UNIT_NAME) values  ('Pieza')</v>
       </c>
@@ -7329,7 +7429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI6"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AA6" sqref="AA6"/>
     </sheetView>
@@ -7366,19 +7466,19 @@
       <c r="D1" s="28"/>
       <c r="E1" s="28"/>
       <c r="F1" s="38"/>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="66" t="s">
         <v>346</v>
       </c>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
       <c r="R1" s="15"/>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
@@ -7680,7 +7780,7 @@
         <f>IF(A6&lt;&gt;"",IF(B6&lt;&gt;"",CONCATENATE(A6,"-",B6),""),"")</f>
         <v>001-MI001</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(AB6," ",AC6," ",AD6," ",AE6," ",AF6," ",AG6," ",AH6," ",AI6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,AA6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @LINEID INT = (SELECT LINE_ID FROM lines WHERE LINE_CODE = '001') DECLARE @CURRENCYID INT = (SELECT CURRENCY_ID FROM currencies WHERE CURRENCY_NAME = 'PESO') DECLARE @ISEXTERNAL BIT = (CASE WHEN 'No' = 'Si' THEN 1 ELSE 0 END) DECLARE @FOBID INT = (SELECT MEASURE_UNIT_ID FROM measure_units WHERE MEASURE_UNIT_NAME ='Caja') DECLARE @CIIFID INT = (SELECT MEASURE_UNIT_ID FROM measure_units WHERE MEASURE_UNIT_NAME ='Centimetro Cúbico') DECLARE @ISPRODNAL BIT = (CASE WHEN 'No' = 'Si' THEN 1 ELSE 0 END) DECLARE @ISACTIVE BIT = (CASE WHEN 'Si' = 'Si' THEN 1 ELSE 0 END) DECLARE @ISVISIBLE BIT = (CASE WHEN 'Si' = 'Si' THEN 1 ELSE 0 END) insert into items (LINE_ID, INTERNAL_REFERENCE, ITEM_NAME, PROVIDER_REFERENCE, PROVIDER_ITEM_NAME, FOB_COST, CURRENCY_ID, NOTES, IS_EXTERNAL_INVENTORY, CIF_COST, VOLUME, WEIGHT, FOB_MEASURE_UNIT_ID, CIF_MEASURE_UNIT_ID, IS_DOMESTIC_PRODUCT, IS_ACTIVE, IS_CATALOG_VISIBLE) values  (@LINEID,'MI001','MI PRUEBA','0001 AZUL','MIPRUEBA PROV',0.1245857,@CURRENCYID,'PRUEBA',@ISEXTERNAL,1,1,1,@FOBID,@CIIFID,@ISPRODNAL,@ISACTIVE,@ISVISIBLE)
 GO</v>
@@ -7867,7 +7967,7 @@
         <f>CONCATENATE("@ITEM_ID",$X$2,"@AREA_ID")</f>
         <v>@ITEM_ID,@AREA_ID</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(N6," ",P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @ITEM_ID INT = (SELECT ITEM_ID FROM items a join lines b on b.LINE_ID = a.LINE_ID WHERE b.LINE_CODE +'-'+a.INTERNAL_REFERENCE = '001-MI001')  DECLARE @AREA_ID SMALLINT = (SELECT AREA_ID FROM areas WHERE AREA_NAME = '001') insert into items_area (ITEM_ID, AREA_ID) values  (@ITEM_ID,@AREA_ID)
 GO</v>
@@ -7878,7 +7978,7 @@
       <c r="P7" s="53"/>
       <c r="Q7" s="23"/>
       <c r="R7" s="53"/>
-      <c r="T7" s="67"/>
+      <c r="T7" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7910,9 +8010,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P2" sqref="P2:Z6"/>
+      <selection pane="bottomLeft" activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7936,18 +8036,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="67" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
       <c r="K1" s="26"/>
       <c r="L1" s="26"/>
       <c r="M1" s="26"/>
@@ -8160,21 +8260,21 @@
         <f>CONCATENATE("@ITEM_ID",$X$2,$W$2,B6,$W$2,$X$2,$W$2,C6,$W$2,$X$2,$W$2,D6,$W$2,$X$2,$W$2,E6,$W$2,$X$2,IF(LEN(F6)&gt;0,CONCATENATE($W$2,F6,$W$2),$Z$2),$X$2,G6+H6,$X$2,"@ISACTIVE",$X$2,J6)</f>
         <v>@ITEM_ID,'004','001AA','Amarillo','Amarillo',NULL,250,@ISACTIVE,100</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE($AA$2," ",P6," ",Q6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),AB6," ",AD6," ",AF6,CHAR(10),"GO")</f>
         <v>DECLARE @LOCAL SMALLINT = (SELECT WAREHOUSE_ID FROM warehouses WHERE WAREHOUSE_CODE = 1) DECLARE @FRANCA SMALLINT = (SELECT WAREHOUSE_ID FROM warehouses WHERE WAREHOUSE_CODE = 2) DECLARE @ITEM_ID INT = (SELECT ITEM_ID FROM items a join lines b on b.LINE_ID = a.LINE_ID WHERE b.LINE_CODE +'-'+a.INTERNAL_REFERENCE = '001-MI001') DECLARE @ISACTIVE BIT = (CASE WHEN 'Si' = 'Si' THEN 1 ELSE 0 END) insert into item_references (ITEM_ID, REFERENCE_CODE, PROVIDER_REFERENCE_CODE, REFERENCE_NAME, PROVIDER_REFERENCE_NAME, NOTES, INVENTORY_QUANTITY, IS_ACTIVE, ALARM_MINIMUM_QUANTITY) values  (@ITEM_ID,'004','001AA','Amarillo','Amarillo',NULL,250,@ISACTIVE,100)
 DECLARE @REFERENCE_ID INT = (SELECT REFERENCE_ID FROM item_references WHERE ITEM_ID = @ITEM_ID AND REFERENCE_CODE = '004') UPDATE references_warehouse set QUANTITY = 200 WHERE WAREHOUSE_ID = @LOCAL AND REFERENCE_ID = @REFERENCE_ID UPDATE references_warehouse set QUANTITY = 50 WHERE WAREHOUSE_ID = @FRANCA AND REFERENCE_ID = @REFERENCE_ID
 GO</v>
       </c>
-      <c r="AB6" s="66" t="str">
+      <c r="AB6" s="58" t="str">
         <f>CONCATENATE("DECLARE @REFERENCE_ID INT = (SELECT REFERENCE_ID FROM item_references WHERE ITEM_ID = @ITEM_ID AND REFERENCE_CODE = '",B6,"')")</f>
         <v>DECLARE @REFERENCE_ID INT = (SELECT REFERENCE_ID FROM item_references WHERE ITEM_ID = @ITEM_ID AND REFERENCE_CODE = '004')</v>
       </c>
-      <c r="AD6" s="66" t="str">
+      <c r="AD6" s="58" t="str">
         <f>CONCATENATE("UPDATE references_warehouse set QUANTITY = ",G6," WHERE WAREHOUSE_ID = @LOCAL AND REFERENCE_ID = @REFERENCE_ID")</f>
         <v>UPDATE references_warehouse set QUANTITY = 200 WHERE WAREHOUSE_ID = @LOCAL AND REFERENCE_ID = @REFERENCE_ID</v>
       </c>
-      <c r="AF6" s="66" t="str">
+      <c r="AF6" s="58" t="str">
         <f>CONCATENATE("UPDATE references_warehouse set QUANTITY = ",H6," WHERE WAREHOUSE_ID = @FRANCA AND REFERENCE_ID = @REFERENCE_ID")</f>
         <v>UPDATE references_warehouse set QUANTITY = 50 WHERE WAREHOUSE_ID = @FRANCA AND REFERENCE_ID = @REFERENCE_ID</v>
       </c>
@@ -8416,7 +8516,7 @@
         <f>CONCATENATE("@IDIDENTTYPE",$X$2,$W$2,B6,$W$2,$X$2,$W$2,C6,$W$2,$X$2,$W$2,D6,$W$2,$X$2,IF(LEN(E6)&gt;0,CONCATENATE($W$2,E6,$W$2),$Z$2),$X$2,IF(LEN(F6)&gt;0,CONCATENATE($W$2,F6,$W$2),$Z$2),$X$2,IF(LEN(G6)&gt;0,CONCATENATE($W$2,G6,$W$2),$Z$2),$X$2,IF(LEN(H6)&gt;0,CONCATENATE($W$2,H6,$W$2),$Z$2),$X$2,IF(LEN(I6)&gt;0,CONCATENATE($W$2,I6,$W$2),$Z$2),$X$2,"@IDCITY")</f>
         <v>@IDIDENTTYPE,'41401793','CARDASOC','Cardenas Asociados','calle 1 a No. 20 -34','300 4525212',NULL,'info@cardasociados.com.co','Francelina Cardenas',@IDCITY</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(P6," ",Q6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDIDENTTYPE INT = (SELECT IDENTITY_TYPE_ID FROM identity_types WHERE IDENTITY_TYPE_CODE =  'NIT') DECLARE @IDCITY INT = (SELECT CITY_ID FROM cities a JOIN departments b ON b.DEPARTMENT_ID = a.DEPARTMENT_ID JOIN countries c ON c.COUNTRY_ID = B.COUNTRY_ID WHERE c.COUNTRY_CODE +'-'+B.DEPARTMENT_NAME+'-'+a.CITY_NAME = 'CO-Cundinamarca-Chia') insert into providers (IDENTITY_TYPE_ID, IDENTITY_NUMBER, PROVIDER_CODE, PROVIDER_NAME, PROVIDER_ADDRESS, PHONE, FAX, EMAIL, CONTACT_PERSON, CITY_ID) values  (@IDIDENTTYPE,'41401793','CARDASOC','Cardenas Asociados','calle 1 a No. 20 -34','300 4525212',NULL,'info@cardasociados.com.co','Francelina Cardenas',@IDCITY)
 GO</v>
@@ -8560,7 +8660,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,$W$2,B6,$W$2,$X$2,IF(LEN(C6)&gt;0,CONCATENATE($W$2,C6,$W$2),$Z$2))</f>
         <v>'001','Despachos',NULL</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2)</f>
         <v>insert into areas (AREA_CODE,AREA_NAME,DESCRIPTION) values  ('001','Despachos',NULL)</v>
       </c>
@@ -8579,7 +8679,7 @@
         <f>CONCATENATE($W$2,A7,$W$2,$X$2,$W$2,B7,$W$2,$X$2,IF(LEN(C7)&gt;0,CONCATENATE($W$2,C7,$W$2),$Z$2))</f>
         <v>'005','Marca Nacional','Servicio al cliente nacional'</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f>CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2)</f>
         <v>insert into areas (AREA_CODE,AREA_NAME,DESCRIPTION) values  ('005','Marca Nacional','Servicio al cliente nacional')</v>
       </c>
@@ -8596,7 +8696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="T6" sqref="T6"/>
     </sheetView>
@@ -8696,7 +8796,7 @@
         <f>CONCATENATE("@REFERENCEID",$X$2,"@PROVIDERID")</f>
         <v>@REFERENCEID,@PROVIDERID</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(N6," ",P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @PROVIDERID INT = (SELECT PROVIDER_ID FROM providers WHERE PROVIDER_CODE = 'CARDASOC') DECLARE @REFERENCEID INT = (SELECT REFERENCE_ID FROM item_references a JOIN items b ON b.ITEM_ID = a.ITEM_ID JOIN lines c ON c.LINE_ID = b.LINE_ID WHERE c.LINE_CODE+'-'+b.INTERNAL_REFERENCE +'-'+a.REFERENCE_CODE = '001-MI001-004') insert into provider_references (REFERENCE_ID, PROVIDER_ID) values  (@REFERENCEID,@PROVIDERID)
 GO</v>
@@ -8707,7 +8807,7 @@
       <c r="P7" s="53"/>
       <c r="Q7" s="23"/>
       <c r="R7" s="53"/>
-      <c r="T7" s="67"/>
+      <c r="T7" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8741,7 +8841,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T6" sqref="T6:T9"/>
+      <selection pane="bottomLeft" sqref="A1:Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8825,7 +8925,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,IF(LEN(B6)&gt;0,CONCATENATE($W$2,B6,$W$2),$Z$2))</f>
         <v>'Coordinadora',NULL</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2)</f>
         <v>insert into shipping_methods (SHIPPING_METHOD_NAME, SHIPPING_METHOD_NOTES) values  ('Coordinadora',NULL)</v>
       </c>
@@ -8838,7 +8938,7 @@
         <f t="shared" ref="R7:R9" si="0">CONCATENATE($W$2,A7,$W$2,$X$2,IF(LEN(B7)&gt;0,CONCATENATE($W$2,B7,$W$2),$Z$2))</f>
         <v>'Servientrega',NULL</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7:T9" si="1">CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2)</f>
         <v>insert into shipping_methods (SHIPPING_METHOD_NAME, SHIPPING_METHOD_NOTES) values  ('Servientrega',NULL)</v>
       </c>
@@ -8851,7 +8951,7 @@
         <f t="shared" si="0"/>
         <v>'Redetrans',NULL</v>
       </c>
-      <c r="T8" s="67" t="str">
+      <c r="T8" s="59" t="str">
         <f t="shared" si="1"/>
         <v>insert into shipping_methods (SHIPPING_METHOD_NAME, SHIPPING_METHOD_NOTES) values  ('Redetrans',NULL)</v>
       </c>
@@ -8864,7 +8964,7 @@
         <f t="shared" si="0"/>
         <v>'Directo',NULL</v>
       </c>
-      <c r="T9" s="67" t="str">
+      <c r="T9" s="59" t="str">
         <f t="shared" si="1"/>
         <v>insert into shipping_methods (SHIPPING_METHOD_NAME, SHIPPING_METHOD_NOTES) values  ('Directo',NULL)</v>
       </c>
@@ -8874,6 +8974,180 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T6" sqref="T6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="13" style="23" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="15"/>
+    <col min="5" max="6" width="11.42578125" style="15" customWidth="1"/>
+    <col min="7" max="14" width="11.42578125" style="15" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="15" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>379</v>
+      </c>
+      <c r="B1" s="28"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="T2" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="U2" s="53" t="s">
+        <v>176</v>
+      </c>
+      <c r="V2" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="W2" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="X2" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y2" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z2" s="53" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="T3" s="53" t="s">
+        <v>381</v>
+      </c>
+      <c r="U3" s="53"/>
+      <c r="V3" s="53" t="s">
+        <v>380</v>
+      </c>
+      <c r="W3" s="53"/>
+      <c r="X3" s="53"/>
+      <c r="Y3" s="53"/>
+      <c r="Z3" s="53"/>
+    </row>
+    <row r="4" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="31"/>
+      <c r="B4" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="68" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" s="69" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="70" t="s">
+        <v>382</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>383</v>
+      </c>
+      <c r="E5" s="70" t="s">
+        <v>384</v>
+      </c>
+      <c r="F5" s="70" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>350</v>
+      </c>
+      <c r="B6" s="71">
+        <v>1.1245000000000001</v>
+      </c>
+      <c r="C6" s="71">
+        <v>1</v>
+      </c>
+      <c r="D6" s="71">
+        <v>1</v>
+      </c>
+      <c r="E6" s="71">
+        <v>1</v>
+      </c>
+      <c r="F6" s="49">
+        <v>100</v>
+      </c>
+      <c r="P6" s="53" t="str">
+        <f>CONCATENATE("DECLARE @ITEM_ID INT = (SELECT ITEM_ID FROM items a join lines b on b.LINE_ID = a.LINE_ID WHERE b.LINE_CODE +'-'+a.INTERNAL_REFERENCE = '",A6,"')")</f>
+        <v>DECLARE @ITEM_ID INT = (SELECT ITEM_ID FROM items a join lines b on b.LINE_ID = a.LINE_ID WHERE b.LINE_CODE +'-'+a.INTERNAL_REFERENCE = '001-MI001')</v>
+      </c>
+      <c r="R6" s="53" t="str">
+        <f>CONCATENATE("@ITEM_ID",$X$2,IF(LEN(B6)&gt;0,B6,$Z$2),$X$2,IF(LEN(C6)&gt;0,C6,$Z$2),$X$2,IF(LEN(D6)&gt;0,D6,$Z$2),$X$2,IF(LEN(E6)&gt;0,E6,$Z$2),$X$2,IF(LEN(F6)&gt;0,F6,$Z$2))</f>
+        <v>@ITEM_ID,1.1245,1,1,1,100</v>
+      </c>
+      <c r="T6" s="59" t="str">
+        <f>CONCATENATE(P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
+        <v>DECLARE @ITEM_ID INT = (SELECT ITEM_ID FROM items a join lines b on b.LINE_ID = a.LINE_ID WHERE b.LINE_CODE +'-'+a.INTERNAL_REFERENCE = '001-MI001') insert into packaging (ITEM_ID, WEIGHT, HEIGHT, WIDTH, LENGTH, QUANTITY) values  (@ITEM_ID,1.1245,1,1,1,100)
+GO</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R7" s="53"/>
+      <c r="T7" s="59"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R8" s="53"/>
+      <c r="T8" s="59"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R9" s="53"/>
+      <c r="T9" s="59"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Articulos!$R$6:$R$100000</xm:f>
+          </x14:formula1>
+          <xm:sqref>A6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -8983,7 +9257,7 @@
         <f>CONCATENATE("@IDACTIVITY",",","@IDAREA")</f>
         <v>@IDACTIVITY,@IDAREA</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(O6," ",P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDACTIVITY SMALLINT = (SELECT ACTIVITY_TYPE_ID FROM activity_types WHERE ACTIVITY_TYPE_NAME = 'Logo Pendiente')  DECLARE @IDAREA SMALLINT = (SELECT AREA_ID FROM areas WHERE AREA_NAME = 'Despachos') insert into activity_types_area (ACTIVITY_TYPE_ID, AREA_ID) values  (@IDACTIVITY,@IDAREA)
 GO</v>
@@ -9008,7 +9282,7 @@
         <f>CONCATENATE("@IDACTIVITY",",","@IDAREA")</f>
         <v>@IDACTIVITY,@IDAREA</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f>CONCATENATE(O7," ",P7," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDACTIVITY SMALLINT = (SELECT ACTIVITY_TYPE_ID FROM activity_types WHERE ACTIVITY_TYPE_NAME = 'Pedido Incompleto')  DECLARE @IDAREA SMALLINT = (SELECT AREA_ID FROM areas WHERE AREA_NAME = 'Marca Nacional') insert into activity_types_area (ACTIVITY_TYPE_ID, AREA_ID) values  (@IDACTIVITY,@IDAREA)
 GO</v>
@@ -9131,7 +9405,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,IF(LEN(C6)&gt;0,CONCATENATE($W$2,C6,$W$2),$Z$2))</f>
         <v>'Dif. Ent. Nacionalización',NULL</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2)</f>
         <v>insert into adjustment_reasons (ADJUSTMENT_REASON_NAME, ADJUSTMENT_REASON_NOTES) values  ('Dif. Ent. Nacionalización',NULL)</v>
       </c>
@@ -9144,7 +9418,7 @@
         <f t="shared" ref="R7:R9" si="0">CONCATENATE($W$2,A7,$W$2,$X$2,IF(LEN(C7)&gt;0,CONCATENATE($W$2,C7,$W$2),$Z$2))</f>
         <v>'Devolución',NULL</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7:T9" si="1">CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2)</f>
         <v>insert into adjustment_reasons (ADJUSTMENT_REASON_NAME, ADJUSTMENT_REASON_NOTES) values  ('Devolución',NULL)</v>
       </c>
@@ -9157,7 +9431,7 @@
         <f t="shared" si="0"/>
         <v>'Producto Defectuoso',NULL</v>
       </c>
-      <c r="T8" s="67" t="str">
+      <c r="T8" s="59" t="str">
         <f t="shared" si="1"/>
         <v>insert into adjustment_reasons (ADJUSTMENT_REASON_NAME, ADJUSTMENT_REASON_NOTES) values  ('Producto Defectuoso',NULL)</v>
       </c>
@@ -9170,7 +9444,7 @@
         <f t="shared" si="0"/>
         <v>'Por Ensamble',NULL</v>
       </c>
-      <c r="T9" s="67" t="str">
+      <c r="T9" s="59" t="str">
         <f t="shared" si="1"/>
         <v>insert into adjustment_reasons (ADJUSTMENT_REASON_NAME, ADJUSTMENT_REASON_NOTES) values  ('Por Ensamble',NULL)</v>
       </c>
@@ -9279,7 +9553,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,IF(B6="Agrega",1,-1))</f>
         <v>'iingresar',1</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2)</f>
         <v>insert into adjustment_types (ADJUSTMENT_TYPE_NAME, OPERATOR) values  ('iingresar',1)</v>
       </c>
@@ -9298,7 +9572,7 @@
         <f>CONCATENATE($W$2,A7,$W$2,$X$2,IF(B7="Agrega",1,-1))</f>
         <v>'retirar',-1</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7" si="0">CONCATENATE($T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2)</f>
         <v>insert into adjustment_types (ADJUSTMENT_TYPE_NAME, OPERATOR) values  ('retirar',-1)</v>
       </c>
@@ -9308,11 +9582,11 @@
         <v>37</v>
       </c>
       <c r="R8" s="53"/>
-      <c r="T8" s="67"/>
+      <c r="T8" s="59"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="R9" s="53"/>
-      <c r="T9" s="67"/>
+      <c r="T9" s="59"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -9447,7 +9721,7 @@
         <f>CONCATENATE("@IDDOCUMENT",$X$2,$W$2,B6,$W$2,$X$2,$W$2,C6,$W$2)</f>
         <v>@IDDOCUMENT,'Alarmas de Ordenes','Alarmas para Ordenes de Compra'</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDDOCUMENT SMALLINT = (SELECT DOCUMENT_TYPE_ID FROM document_types WHERE DOCUMENT_TYPE_NAME = 'Orden') insert into alarm_types (DOCUMENT_TYPE_ID, NAME, DESCRIPTION) values  (@IDDOCUMENT,'Alarmas de Ordenes','Alarmas para Ordenes de Compra')
 GO</v>
@@ -9474,7 +9748,7 @@
         <f t="shared" ref="R7:R8" si="1">CONCATENATE("@IDDOCUMENT",$X$2,$W$2,B7,$W$2,$X$2,$W$2,C7,$W$2)</f>
         <v>@IDDOCUMENT,'Alarmas de Pedidos','Alarmas para Pedidos'</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7:T8" si="2">CONCATENATE(P7," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDDOCUMENT SMALLINT = (SELECT DOCUMENT_TYPE_ID FROM document_types WHERE DOCUMENT_TYPE_NAME = 'Pedido') insert into alarm_types (DOCUMENT_TYPE_ID, NAME, DESCRIPTION) values  (@IDDOCUMENT,'Alarmas de Pedidos','Alarmas para Pedidos')
 GO</v>
@@ -9501,7 +9775,7 @@
         <f t="shared" si="1"/>
         <v>@IDDOCUMENT,'Alarmas de Reservas','Alarmas para Reservas'</v>
       </c>
-      <c r="T8" s="67" t="str">
+      <c r="T8" s="59" t="str">
         <f t="shared" si="2"/>
         <v>DECLARE @IDDOCUMENT SMALLINT = (SELECT DOCUMENT_TYPE_ID FROM document_types WHERE DOCUMENT_TYPE_NAME = 'Reserva') insert into alarm_types (DOCUMENT_TYPE_ID, NAME, DESCRIPTION) values  (@IDDOCUMENT,'Alarmas de Reservas','Alarmas para Reservas')
 GO</v>
@@ -9510,7 +9784,7 @@
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="P9" s="53"/>
       <c r="R9" s="53"/>
-      <c r="T9" s="67"/>
+      <c r="T9" s="59"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -9625,7 +9899,7 @@
         <f>CONCATENATE("@IDALARMTYPE",$X$2,$W$2,B6,$W$2)</f>
         <v>@IDALARMTYPE,'Revisar estado de importacion'</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDALARMTYPE SMALLINT = (SELECT ALARM_TYPE_ID FROM alarm_types WHERE NAME = 'Alarmas de Ordenes') insert into alarm_messages (ALARM_TYPE_ID, ALARM_MESSAGE) values  (@IDALARMTYPE,'Revisar estado de importacion')
 GO</v>
@@ -9646,7 +9920,7 @@
         <f t="shared" ref="R7" si="1">CONCATENATE("@IDALARMTYPE",$X$2,$W$2,B7,$W$2)</f>
         <v>@IDALARMTYPE,'Confirmar Marcacion de Articulos'</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7" si="2">CONCATENATE(P7," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDALARMTYPE SMALLINT = (SELECT ALARM_TYPE_ID FROM alarm_types WHERE NAME = 'Alarmas de Pedidos') insert into alarm_messages (ALARM_TYPE_ID, ALARM_MESSAGE) values  (@IDALARMTYPE,'Confirmar Marcacion de Articulos')
 GO</v>
@@ -9655,7 +9929,7 @@
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="P8" s="53"/>
       <c r="R8" s="53"/>
-      <c r="T8" s="67"/>
+      <c r="T8" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9787,7 +10061,7 @@
         <f>CONCATENATE($W$2,A6,$W$2,$X$2,"@IDDOCUMENT",$X$2,IF(LEN(C6)&gt;0,CONCATENATE($W$2,C6,$W$2),$Z$2))</f>
         <v>'solicitud del cliente',@IDDOCUMENT,NULL</v>
       </c>
-      <c r="T6" s="67" t="str">
+      <c r="T6" s="59" t="str">
         <f>CONCATENATE(P6," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R6,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDDOCUMENT SMALLINT = (SELECT DOCUMENT_TYPE_ID FROM document_types WHERE DOCUMENT_TYPE_NAME = 'Pedido') insert into cancellation_reasons (CANCELLATION_REASON_NAME, DOCUMENT_TYPE_ID, NOTES) values  ('solicitud del cliente',@IDDOCUMENT,NULL)
 GO</v>
@@ -9814,7 +10088,7 @@
         <f t="shared" ref="R7:R8" si="1">CONCATENATE($W$2,A7,$W$2,$X$2,"@IDDOCUMENT",$X$2,IF(LEN(C7)&gt;0,CONCATENATE($W$2,C7,$W$2),$Z$2))</f>
         <v>'Inventario Insuficiente',@IDDOCUMENT,'Proveedor no cuenta con los Articulos solicitados'</v>
       </c>
-      <c r="T7" s="67" t="str">
+      <c r="T7" s="59" t="str">
         <f t="shared" ref="T7:T8" si="2">CONCATENATE(P7," ",$T$2,$T$3,$V$2,$V$3,$Y$2,$U$2,$V$2,R7,$Y$2,CHAR(10),"GO")</f>
         <v>DECLARE @IDDOCUMENT SMALLINT = (SELECT DOCUMENT_TYPE_ID FROM document_types WHERE DOCUMENT_TYPE_NAME = 'Orden') insert into cancellation_reasons (CANCELLATION_REASON_NAME, DOCUMENT_TYPE_ID, NOTES) values  ('Inventario Insuficiente',@IDDOCUMENT,'Proveedor no cuenta con los Articulos solicitados')
 GO</v>
@@ -9838,7 +10112,7 @@
         <f t="shared" si="1"/>
         <v>'Cancelado por el cliente',@IDDOCUMENT,NULL</v>
       </c>
-      <c r="T8" s="67" t="str">
+      <c r="T8" s="59" t="str">
         <f t="shared" si="2"/>
         <v>DECLARE @IDDOCUMENT SMALLINT = (SELECT DOCUMENT_TYPE_ID FROM document_types WHERE DOCUMENT_TYPE_NAME = 'Reserva') insert into cancellation_reasons (CANCELLATION_REASON_NAME, DOCUMENT_TYPE_ID, NOTES) values  ('Cancelado por el cliente',@IDDOCUMENT,NULL)
 GO</v>

</xml_diff>